<commit_message>
[Jimmy] merge de cambios de diapositivas de puntos clientes
</commit_message>
<xml_diff>
--- a/src/assets/anexos/cargar_bigpuntos_corp.xlsx
+++ b/src/assets/anexos/cargar_bigpuntos_corp.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/grp-general-ifi-front-corp/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F38B1D9-0C0A-6D42-B194-26F0132995AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE239083-4457-C14C-B4A7-E756D7187262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51200" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{3FDAB71D-9125-44FE-8F2C-4B501D5972E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Empleados" sheetId="1" r:id="rId1"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -195,7 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -205,7 +205,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -533,7 +532,7 @@
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.83203125" style="1"/>
     <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="8" max="8" width="26.5" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>